<commit_message>
modifique un archivo 2rama.xlsx
</commit_message>
<xml_diff>
--- a/2rama.xlsx
+++ b/2rama.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -16,8 +16,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +54,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Oficina">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,9 +106,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Oficina">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -132,9 +140,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +175,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Oficina">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,38 +351,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>